<commit_message>
selenium and pytest practise
</commit_message>
<xml_diff>
--- a/Deepesh/AutomationFramework/utilities/sample.xlsx
+++ b/Deepesh/AutomationFramework/utilities/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trainings\GTM_PS_Batch11_26May25\GTM_PS_BATCH11\Deepesh\AutomationFramework\utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonAutomation\GTM_PS_BATCH11\Deepesh\AutomationFramework\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BF7669-7E28-41CA-8D44-CA9116CBA08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E56DE36-CCFA-481F-B738-1468FEF1EC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>